<commit_message>
Update .gitignore to exclude VSCode settings and add keyword dictionary resource
</commit_message>
<xml_diff>
--- a/resources/keyword_dict_annotated_expanded.xlsx
+++ b/resources/keyword_dict_annotated_expanded.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C517"/>
+  <dimension ref="A1:C513"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3921,7 +3921,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>discharge</t>
+          <t>elimination</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -3931,14 +3931,14 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>discharge</t>
+          <t>elimination</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>discharged</t>
+          <t>eliminations</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -3948,14 +3948,14 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>discharge</t>
+          <t>elimination</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>discharges</t>
+          <t>fecal_matter</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -3965,14 +3965,14 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>discharge</t>
+          <t>fecal_matter</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>discharging</t>
+          <t>fecal_mattered</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -3982,14 +3982,14 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>discharge</t>
+          <t>fecal_matter</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>elimination</t>
+          <t>fecal_mattering</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -3999,14 +3999,14 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>elimination</t>
+          <t>fecal_matter</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>eliminations</t>
+          <t>fecal_matters</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -4016,14 +4016,14 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>elimination</t>
+          <t>fecal_matter</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>fecal_matter</t>
+          <t>fecula</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -4033,14 +4033,14 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>fecal_matter</t>
+          <t>fecula</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>fecal_mattered</t>
+          <t>feculas</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -4050,14 +4050,14 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>fecal_matter</t>
+          <t>fecula</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>fecal_mattering</t>
+          <t>guano</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -4067,14 +4067,14 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>fecal_matter</t>
+          <t>guano</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>fecal_matters</t>
+          <t>guanos</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -4084,14 +4084,14 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>fecal_matter</t>
+          <t>guano</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>fecula</t>
+          <t>human_waste</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4101,14 +4101,14 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>fecula</t>
+          <t>human_waste</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>feculas</t>
+          <t>human_wasted</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -4118,14 +4118,14 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>fecula</t>
+          <t>human_waste</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>guano</t>
+          <t>human_wastes</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4135,14 +4135,14 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>guano</t>
+          <t>human_waste</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>guanos</t>
+          <t>human_wasting</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -4152,14 +4152,14 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>guano</t>
+          <t>human_waste</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>human_waste</t>
+          <t>humans_waste</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -4176,7 +4176,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>human_wasted</t>
+          <t>humans_wasted</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -4193,7 +4193,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>human_wastes</t>
+          <t>humans_wastes</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>human_wasting</t>
+          <t>humans_wasting</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -4227,7 +4227,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>humans_waste</t>
+          <t>incontinence</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4237,14 +4237,14 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>human_waste</t>
+          <t>incontinence</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>humans_wasted</t>
+          <t>incontinences</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -4254,14 +4254,14 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>human_waste</t>
+          <t>incontinence</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>humans_wastes</t>
+          <t>micturition</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -4271,14 +4271,14 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>human_waste</t>
+          <t>micturition</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>humans_wasting</t>
+          <t>micturitions</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -4288,14 +4288,14 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>human_waste</t>
+          <t>micturition</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>incontinence</t>
+          <t>urine</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4305,14 +4305,14 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>incontinence</t>
+          <t>urine</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>incontinences</t>
+          <t>urines</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -4322,14 +4322,14 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>incontinence</t>
+          <t>urine</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>micturition</t>
+          <t>waste</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -4339,14 +4339,14 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>micturition</t>
+          <t>waste</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>micturitions</t>
+          <t>wasted</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -4356,14 +4356,14 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>micturition</t>
+          <t>waste</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>urine</t>
+          <t>wastes</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -4373,14 +4373,14 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>urine</t>
+          <t>waste</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>urines</t>
+          <t>wasting</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -4390,82 +4390,82 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>urine</t>
+          <t>waste</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>waste</t>
+          <t>aunt</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Excretion</t>
+          <t>Family</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>waste</t>
+          <t>aunt</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>wasted</t>
+          <t>aunts</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Excretion</t>
+          <t>Family</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>waste</t>
+          <t>aunt</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>wastes</t>
+          <t>brethren</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Excretion</t>
+          <t>Family</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>waste</t>
+          <t>brother</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>wasting</t>
+          <t>brother</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Excretion</t>
+          <t>Family</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>waste</t>
+          <t>brother</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>aunt</t>
+          <t>brothers</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4475,14 +4475,14 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>aunt</t>
+          <t>brother</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>aunts</t>
+          <t>couple</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -4492,14 +4492,14 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>aunt</t>
+          <t>couple</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>brethren</t>
+          <t>coupled</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -4509,14 +4509,14 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>brother</t>
+          <t>couple</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>brother</t>
+          <t>couples</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -4526,14 +4526,14 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>brother</t>
+          <t>couple</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>brothers</t>
+          <t>coupling</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -4543,14 +4543,14 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>brother</t>
+          <t>couple</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>couple</t>
+          <t>daughter</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4560,14 +4560,14 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>couple</t>
+          <t>daughter</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>coupled</t>
+          <t>daughters</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -4577,14 +4577,14 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>couple</t>
+          <t>daughter</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>couples</t>
+          <t>families</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -4594,14 +4594,14 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>couple</t>
+          <t>family</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>coupling</t>
+          <t>family</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -4611,14 +4611,14 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>couple</t>
+          <t>family</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>daughter</t>
+          <t>father</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4628,14 +4628,14 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>daughter</t>
+          <t>father</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>daughters</t>
+          <t>fathered</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -4645,14 +4645,14 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>daughter</t>
+          <t>father</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>families</t>
+          <t>fathering</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -4662,14 +4662,14 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>father</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>fathers</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -4679,14 +4679,14 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>father</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>father</t>
+          <t>foster_families</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -4696,14 +4696,14 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>father</t>
+          <t>foster_family</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>fathered</t>
+          <t>foster_family</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -4713,14 +4713,14 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>father</t>
+          <t>foster_family</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>fathering</t>
+          <t>fostered_families</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -4730,14 +4730,14 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>father</t>
+          <t>foster_family</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>fathers</t>
+          <t>fostered_family</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -4747,14 +4747,14 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>father</t>
+          <t>foster_family</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>foster_families</t>
+          <t>fostering_families</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -4771,7 +4771,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>foster_family</t>
+          <t>fostering_family</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -4788,7 +4788,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>fostered_families</t>
+          <t>fosters_families</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -4805,7 +4805,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>fostered_family</t>
+          <t>fosters_family</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>fostering_families</t>
+          <t>husband</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -4832,14 +4832,14 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>foster_family</t>
+          <t>husband</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>fostering_family</t>
+          <t>husbanded</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -4849,14 +4849,14 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>foster_family</t>
+          <t>husband</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>fosters_families</t>
+          <t>husbanding</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -4866,14 +4866,14 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>foster_family</t>
+          <t>husband</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>fosters_family</t>
+          <t>husbands</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -4883,14 +4883,14 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>foster_family</t>
+          <t>husband</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>husband</t>
+          <t>kin</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -4900,14 +4900,14 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>husband</t>
+          <t>kin</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>husbanded</t>
+          <t>kins</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -4917,14 +4917,14 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>husband</t>
+          <t>kin</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>husbanding</t>
+          <t>mother</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -4934,14 +4934,14 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>husband</t>
+          <t>mother</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>husbands</t>
+          <t>mothered</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -4951,14 +4951,14 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>husband</t>
+          <t>mother</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>kin</t>
+          <t>mothering</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -4968,14 +4968,14 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>kin</t>
+          <t>mother</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>kins</t>
+          <t>mothers</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -4985,14 +4985,14 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>kin</t>
+          <t>mother</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>relative</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -5002,14 +5002,14 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>relative</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>mothered</t>
+          <t>relatives</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -5019,14 +5019,14 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>relative</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>mothering</t>
+          <t>sister</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -5036,14 +5036,14 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>sister</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>mothers</t>
+          <t>sisters</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -5053,14 +5053,14 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>sister</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>relative</t>
+          <t>son</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -5070,14 +5070,14 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>relative</t>
+          <t>son</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>relatives</t>
+          <t>sons</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -5087,14 +5087,14 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>relative</t>
+          <t>son</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>sister</t>
+          <t>uncle</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -5104,14 +5104,14 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>sister</t>
+          <t>uncle</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>sisters</t>
+          <t>uncles</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -5121,82 +5121,82 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>sister</t>
+          <t>uncle</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>son</t>
+          <t>alert</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Family</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>son</t>
+          <t>alert</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>sons</t>
+          <t>alerted</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Family</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>son</t>
+          <t>alert</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>uncle</t>
+          <t>alerting</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Family</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>uncle</t>
+          <t>alert</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>uncles</t>
+          <t>alerts</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Family</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>uncle</t>
+          <t>alert</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>alert</t>
+          <t>orient</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -5206,14 +5206,14 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>alert</t>
+          <t>orient</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>alerted</t>
+          <t>oriented</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -5223,14 +5223,14 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>alert</t>
+          <t>orient</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>alerting</t>
+          <t>orienting</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -5240,14 +5240,14 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>alert</t>
+          <t>orient</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>alerts</t>
+          <t>orients</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -5257,82 +5257,82 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>alert</t>
+          <t>orient</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>orient</t>
+          <t>ache</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Pain</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>orient</t>
+          <t>ache</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>oriented</t>
+          <t>ached</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Pain</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>orient</t>
+          <t>ache</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>orienting</t>
+          <t>aches</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Pain</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>orient</t>
+          <t>ache</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>orients</t>
+          <t>aching</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Pain</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>orient</t>
+          <t>ache</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>ache</t>
+          <t>agonies</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -5342,14 +5342,14 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>ache</t>
+          <t>agony</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>ached</t>
+          <t>agonize</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -5359,14 +5359,14 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>ache</t>
+          <t>agonize</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>aches</t>
+          <t>agonized</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -5376,14 +5376,14 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>ache</t>
+          <t>agonize</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>aching</t>
+          <t>agonizes</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -5393,14 +5393,14 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>ache</t>
+          <t>agonize</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>agonies</t>
+          <t>agonizing</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -5410,14 +5410,14 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>agony</t>
+          <t>agonize</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>agonize</t>
+          <t>agony</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -5427,14 +5427,14 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>agonize</t>
+          <t>agony</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>agonized</t>
+          <t>arthralgia</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -5444,14 +5444,14 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>agonize</t>
+          <t>arthralgia</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>agonizes</t>
+          <t>arthralgias</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -5461,14 +5461,14 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>agonize</t>
+          <t>arthralgia</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>agonizing</t>
+          <t>burn</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -5478,14 +5478,14 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>agonize</t>
+          <t>burn</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>agony</t>
+          <t>burned</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -5495,14 +5495,14 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>agony</t>
+          <t>burn</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>arthralgia</t>
+          <t>burning</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -5512,14 +5512,14 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>arthralgia</t>
+          <t>burn</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>arthralgias</t>
+          <t>burns</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -5529,14 +5529,14 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>arthralgia</t>
+          <t>burn</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>burn</t>
+          <t>burnt</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -5553,7 +5553,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>burned</t>
+          <t>causalgia</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -5563,14 +5563,14 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>burn</t>
+          <t>causalgia</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>burning</t>
+          <t>causalgias</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -5580,14 +5580,14 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>burn</t>
+          <t>causalgia</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>burns</t>
+          <t>chiralgia</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -5597,14 +5597,14 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>burn</t>
+          <t>chiralgia</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>burnt</t>
+          <t>chiralgias</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -5614,14 +5614,14 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>burn</t>
+          <t>chiralgia</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>causalgia</t>
+          <t>colic</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -5631,14 +5631,14 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>causalgia</t>
+          <t>colic</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>causalgias</t>
+          <t>colics</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -5648,14 +5648,14 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>causalgia</t>
+          <t>colic</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>chiralgia</t>
+          <t>distress</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -5665,14 +5665,14 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>chiralgia</t>
+          <t>distress</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>chiralgias</t>
+          <t>distressed</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -5682,14 +5682,14 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>chiralgia</t>
+          <t>distress</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>colic</t>
+          <t>distresses</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -5699,14 +5699,14 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>colic</t>
+          <t>distress</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>colics</t>
+          <t>distressing</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -5716,14 +5716,14 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>colic</t>
+          <t>distress</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>distress</t>
+          <t>dysmenorrhea</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -5733,14 +5733,14 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>distress</t>
+          <t>dysmenorrhea</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>distressed</t>
+          <t>dysmenorrheas</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -5750,14 +5750,14 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>distress</t>
+          <t>dysmenorrhea</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>distresses</t>
+          <t>glossalgia</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -5767,14 +5767,14 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>distress</t>
+          <t>glossalgia</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>distressing</t>
+          <t>glossalgias</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -5784,14 +5784,14 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>distress</t>
+          <t>glossalgia</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>dysmenorrhea</t>
+          <t>grew_pain</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -5801,14 +5801,14 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>dysmenorrhea</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>dysmenorrheas</t>
+          <t>grew_pained</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -5818,14 +5818,14 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>dysmenorrhea</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>glossalgia</t>
+          <t>grew_paining</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -5835,14 +5835,14 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>glossalgia</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>glossalgias</t>
+          <t>grew_pains</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -5852,14 +5852,14 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>glossalgia</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>grew_pain</t>
+          <t>grew_pains</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -5869,14 +5869,14 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>grew_pained</t>
+          <t>grew_painss</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -5886,14 +5886,14 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>grew_paining</t>
+          <t>grow_pain</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -5910,7 +5910,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>grew_pains</t>
+          <t>grow_pained</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -5927,7 +5927,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>grew_pains</t>
+          <t>grow_paining</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -5937,14 +5937,14 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>grew_painss</t>
+          <t>grow_pains</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -5954,14 +5954,14 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -5971,14 +5971,14 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>grow_pained</t>
+          <t>grow_painss</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -5988,14 +5988,14 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>grow_paining</t>
+          <t>growing_pain</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -6012,7 +6012,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>growing_pain</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -6022,14 +6022,14 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>growing_pain</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>growing_pained</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -6039,14 +6039,14 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>grow_painss</t>
+          <t>growing_pained</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -6056,14 +6056,14 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>growing_pain</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>growing_paining</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -6080,7 +6080,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>growing_paining</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -6097,7 +6097,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>growing_pained</t>
+          <t>growing_pains</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -6114,7 +6114,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>growing_pained</t>
+          <t>growing_pains</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -6124,14 +6124,14 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>growing_paining</t>
+          <t>growing_pains</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -6141,14 +6141,14 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>growing_pain</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>growing_paining</t>
+          <t>growing_pains</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -6158,14 +6158,14 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>growing_pains</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>growing_painss</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -6175,31 +6175,31 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
+          <t>growing_painss</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Pain</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
           <t>growing_pains</t>
-        </is>
-      </c>
-      <c r="B339" t="inlineStr">
-        <is>
-          <t>Pain</t>
-        </is>
-      </c>
-      <c r="C339" t="inlineStr">
-        <is>
-          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>growings_pain</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -6216,7 +6216,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>growings_pained</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -6226,14 +6226,14 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>growing_pain</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>growing_painss</t>
+          <t>growings_paining</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -6243,14 +6243,14 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>growing_pain</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>growing_painss</t>
+          <t>growings_pains</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -6260,14 +6260,14 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>growing_pain</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>growings_pain</t>
+          <t>growings_pains</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -6277,14 +6277,14 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>growing_pains</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>growings_pained</t>
+          <t>growings_painss</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -6294,14 +6294,14 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>growing_pains</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>growings_paining</t>
+          <t>grown_pain</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -6311,14 +6311,14 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>growings_pains</t>
+          <t>grown_pained</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -6328,14 +6328,14 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>growing_pain</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>growings_pains</t>
+          <t>grown_paining</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -6345,14 +6345,14 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>growings_painss</t>
+          <t>grown_pains</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -6362,14 +6362,14 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>growing_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>grown_pain</t>
+          <t>grown_pains</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -6379,14 +6379,14 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>grown_pained</t>
+          <t>grown_painss</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -6396,14 +6396,14 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>grown_paining</t>
+          <t>grows_pain</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -6420,7 +6420,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>grown_pains</t>
+          <t>grows_pained</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -6437,7 +6437,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>grown_pains</t>
+          <t>grows_paining</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -6447,14 +6447,14 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>grown_painss</t>
+          <t>grows_pains</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -6464,14 +6464,14 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>grow_pain</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>grows_pain</t>
+          <t>grows_pains</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -6481,14 +6481,14 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>grows_pained</t>
+          <t>grows_painss</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -6498,14 +6498,14 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>grow_pains</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>grows_paining</t>
+          <t>hemorrhoid</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -6515,14 +6515,14 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>hemorrhoid</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>grows_pains</t>
+          <t>hemorrhoids</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -6532,14 +6532,14 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>grow_pain</t>
+          <t>hemorrhoid</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>grows_pains</t>
+          <t>keratalgia</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -6549,14 +6549,14 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>keratalgia</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>grows_painss</t>
+          <t>keratalgias</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -6566,14 +6566,14 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>grow_pains</t>
+          <t>keratalgia</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>hemorrhoid</t>
+          <t>labor_pain</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -6583,14 +6583,14 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>hemorrhoid</t>
+          <t>labor_pain</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>hemorrhoids</t>
+          <t>labor_pained</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -6600,14 +6600,14 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>hemorrhoid</t>
+          <t>labor_pain</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>keratalgia</t>
+          <t>labor_paining</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -6617,14 +6617,14 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>keratalgia</t>
+          <t>labor_pain</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>keratalgias</t>
+          <t>labor_pains</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -6634,14 +6634,14 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>keratalgia</t>
+          <t>labor_pain</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>labor_pain</t>
+          <t>labors_pain</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -6658,7 +6658,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>labor_pained</t>
+          <t>labors_pained</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -6675,7 +6675,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>labor_paining</t>
+          <t>labors_paining</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -6692,7 +6692,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>labor_pains</t>
+          <t>labors_pains</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>labors_pain</t>
+          <t>mastalgia</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -6719,14 +6719,14 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>labor_pain</t>
+          <t>mastalgia</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>labors_pained</t>
+          <t>mastalgias</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -6736,14 +6736,14 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>labor_pain</t>
+          <t>mastalgia</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>labors_paining</t>
+          <t>melagra</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -6753,14 +6753,14 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>labor_pain</t>
+          <t>melagra</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>labors_pains</t>
+          <t>melagras</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -6770,14 +6770,14 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>labor_pain</t>
+          <t>melagra</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>mastalgia</t>
+          <t>meralgia</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -6787,14 +6787,14 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>mastalgia</t>
+          <t>meralgia</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>mastalgias</t>
+          <t>meralgias</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -6804,14 +6804,14 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>mastalgia</t>
+          <t>meralgia</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>melagra</t>
+          <t>metralgia</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -6821,14 +6821,14 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>melagra</t>
+          <t>metralgia</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>melagras</t>
+          <t>metralgias</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -6838,14 +6838,14 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>melagra</t>
+          <t>metralgia</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>meralgia</t>
+          <t>mittelschmerz</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -6855,14 +6855,14 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>meralgia</t>
+          <t>mittelschmerz</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>meralgias</t>
+          <t>mittelschmerzs</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -6872,14 +6872,14 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>meralgia</t>
+          <t>mittelschmerz</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>metralgia</t>
+          <t>myalgia</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -6889,14 +6889,14 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>metralgia</t>
+          <t>myalgia</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>metralgias</t>
+          <t>myalgias</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -6906,14 +6906,14 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>metralgia</t>
+          <t>myalgia</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>mittelschmerz</t>
+          <t>nephralgia</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -6923,14 +6923,14 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>mittelschmerz</t>
+          <t>nephralgia</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>mittelschmerzs</t>
+          <t>nephralgias</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -6940,14 +6940,14 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>mittelschmerz</t>
+          <t>nephralgia</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>myalgia</t>
+          <t>neuralgia</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -6957,14 +6957,14 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>myalgia</t>
+          <t>neuralgia</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>myalgias</t>
+          <t>neuralgias</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -6974,14 +6974,14 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>myalgia</t>
+          <t>neuralgia</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>nephralgia</t>
+          <t>odynophagia</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -6991,14 +6991,14 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>nephralgia</t>
+          <t>odynophagia</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>nephralgias</t>
+          <t>odynophagias</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -7008,14 +7008,14 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>nephralgia</t>
+          <t>odynophagia</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>neuralgia</t>
+          <t>orchidalgia</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -7025,14 +7025,14 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>neuralgia</t>
+          <t>orchidalgia</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>neuralgias</t>
+          <t>orchidalgias</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -7042,14 +7042,14 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>neuralgia</t>
+          <t>orchidalgia</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>odynophagia</t>
+          <t>pain</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
@@ -7059,14 +7059,14 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>odynophagia</t>
+          <t>pain</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>odynophagias</t>
+          <t>pained</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -7076,14 +7076,14 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>odynophagia</t>
+          <t>pain</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>orchidalgia</t>
+          <t>paining</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -7093,14 +7093,14 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>orchidalgia</t>
+          <t>pain</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>orchidalgias</t>
+          <t>pains</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -7110,14 +7110,14 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>orchidalgia</t>
+          <t>pain</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>pain</t>
+          <t>pang</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
@@ -7127,14 +7127,14 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>pain</t>
+          <t>pang</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>pained</t>
+          <t>pangs</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -7144,14 +7144,14 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>pain</t>
+          <t>pang</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>paining</t>
+          <t>phantom_limb_pain</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -7161,14 +7161,14 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>pain</t>
+          <t>phantom_limb_pain</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>pains</t>
+          <t>phantom_limb_pained</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -7178,14 +7178,14 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>pain</t>
+          <t>phantom_limb_pain</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>pang</t>
+          <t>phantom_limb_paining</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -7195,14 +7195,14 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>pang</t>
+          <t>phantom_limb_pain</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>pangs</t>
+          <t>phantom_limb_pains</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -7212,14 +7212,14 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>pang</t>
+          <t>phantom_limb_pain</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>phantom_limb_pain</t>
+          <t>phantom_limbed_pain</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
@@ -7236,7 +7236,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>phantom_limb_pained</t>
+          <t>phantom_limbed_pained</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
@@ -7253,7 +7253,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>phantom_limb_paining</t>
+          <t>phantom_limbed_paining</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -7270,7 +7270,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>phantom_limb_pains</t>
+          <t>phantom_limbed_pains</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -7287,7 +7287,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>phantom_limbed_pain</t>
+          <t>phantom_limbs_pain</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -7304,7 +7304,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>phantom_limbed_pained</t>
+          <t>phantom_limbs_pained</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -7321,7 +7321,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>phantom_limbed_paining</t>
+          <t>phantom_limbs_paining</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -7338,7 +7338,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>phantom_limbed_pains</t>
+          <t>phantom_limbs_pains</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -7355,7 +7355,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>phantom_limbs_pain</t>
+          <t>phantoms_limb_pain</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -7372,7 +7372,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>phantom_limbs_pained</t>
+          <t>phantoms_limb_pained</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -7389,7 +7389,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>phantom_limbs_paining</t>
+          <t>phantoms_limb_paining</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -7406,7 +7406,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>phantom_limbs_pains</t>
+          <t>phantoms_limb_pains</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -7423,7 +7423,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>phantoms_limb_pain</t>
+          <t>phantoms_limbed_pain</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -7440,7 +7440,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>phantoms_limb_pained</t>
+          <t>phantoms_limbed_pained</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -7457,7 +7457,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>phantoms_limb_paining</t>
+          <t>phantoms_limbed_paining</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
@@ -7474,7 +7474,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>phantoms_limb_pains</t>
+          <t>phantoms_limbed_pains</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
@@ -7491,7 +7491,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>phantoms_limbed_pain</t>
+          <t>phantoms_limbs_pain</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
@@ -7508,7 +7508,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>phantoms_limbed_pained</t>
+          <t>phantoms_limbs_pained</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -7525,7 +7525,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>phantoms_limbed_paining</t>
+          <t>phantoms_limbs_paining</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -7542,7 +7542,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>phantoms_limbed_pains</t>
+          <t>phantoms_limbs_pains</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
@@ -7559,7 +7559,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>phantoms_limbs_pain</t>
+          <t>photalgia</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
@@ -7569,14 +7569,14 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>phantom_limb_pain</t>
+          <t>photalgia</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>phantoms_limbs_pained</t>
+          <t>photalgias</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
@@ -7586,14 +7586,14 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>phantom_limb_pain</t>
+          <t>photalgia</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>phantoms_limbs_paining</t>
+          <t>pleurodynia</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
@@ -7603,14 +7603,14 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>phantom_limb_pain</t>
+          <t>pleurodynia</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>phantoms_limbs_pains</t>
+          <t>pleurodynias</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -7620,14 +7620,14 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>phantom_limb_pain</t>
+          <t>pleurodynia</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>photalgia</t>
+          <t>podalgia</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
@@ -7637,14 +7637,14 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>photalgia</t>
+          <t>podalgia</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>photalgias</t>
+          <t>podalgias</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -7654,14 +7654,14 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>photalgia</t>
+          <t>podalgia</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>pleurodynia</t>
+          <t>proctalgia</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -7671,14 +7671,14 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>pleurodynia</t>
+          <t>proctalgia</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>pleurodynias</t>
+          <t>proctalgias</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -7688,14 +7688,14 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>pleurodynia</t>
+          <t>proctalgia</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>podalgia</t>
+          <t>refer_pain</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -7705,14 +7705,14 @@
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>podalgia</t>
+          <t>refer_pain</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>podalgias</t>
+          <t>refer_pained</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
@@ -7722,14 +7722,14 @@
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>podalgia</t>
+          <t>refer_pain</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>proctalgia</t>
+          <t>refer_paining</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -7739,14 +7739,14 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>proctalgia</t>
+          <t>refer_pain</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>proctalgias</t>
+          <t>refer_pains</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -7756,14 +7756,14 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>proctalgia</t>
+          <t>refer_pain</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>refer_pain</t>
+          <t>referred_pain</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -7780,7 +7780,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>refer_pained</t>
+          <t>referred_pained</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -7797,7 +7797,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>refer_paining</t>
+          <t>referred_paining</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -7814,7 +7814,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>refer_pains</t>
+          <t>referred_pains</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -7831,7 +7831,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>referred_pain</t>
+          <t>referring_pain</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
@@ -7848,7 +7848,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>referred_pained</t>
+          <t>referring_pained</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
@@ -7865,7 +7865,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>referred_paining</t>
+          <t>referring_paining</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
@@ -7882,7 +7882,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>referred_pains</t>
+          <t>referring_pains</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -7899,7 +7899,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>referring_pain</t>
+          <t>refers_pain</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -7916,7 +7916,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>referring_pained</t>
+          <t>refers_pained</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
@@ -7933,7 +7933,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>referring_paining</t>
+          <t>refers_paining</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -7950,7 +7950,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>referring_pains</t>
+          <t>refers_pains</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -7967,7 +7967,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>refers_pain</t>
+          <t>renal_colic</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -7977,14 +7977,14 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>refer_pain</t>
+          <t>renal_colic</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>refers_pained</t>
+          <t>renal_colics</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -7994,14 +7994,14 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>refer_pain</t>
+          <t>renal_colic</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>refers_paining</t>
+          <t>smart</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -8011,14 +8011,14 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>refer_pain</t>
+          <t>smart</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>refers_pains</t>
+          <t>smarted</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -8028,14 +8028,14 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>refer_pain</t>
+          <t>smart</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>renal_colic</t>
+          <t>smarter</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
@@ -8045,14 +8045,14 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>renal_colic</t>
+          <t>smart</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>renal_colics</t>
+          <t>smartest</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -8062,14 +8062,14 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>renal_colic</t>
+          <t>smart</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>smart</t>
+          <t>smarting</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -8086,7 +8086,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>smarted</t>
+          <t>smarts</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -8103,7 +8103,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>smarter</t>
+          <t>somesthesia</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -8113,14 +8113,14 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>smart</t>
+          <t>somesthesia</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>smartest</t>
+          <t>somesthesias</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -8130,14 +8130,14 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>smart</t>
+          <t>somesthesia</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>smarting</t>
+          <t>sting</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
@@ -8147,14 +8147,14 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>smart</t>
+          <t>sting</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>smarts</t>
+          <t>stinging</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
@@ -8164,14 +8164,14 @@
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>smart</t>
+          <t>sting</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>somesthesia</t>
+          <t>stings</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -8181,14 +8181,14 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>somesthesia</t>
+          <t>sting</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>somesthesias</t>
+          <t>stitch</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -8198,14 +8198,14 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>somesthesia</t>
+          <t>stitch</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>sting</t>
+          <t>stitched</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -8215,14 +8215,14 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>sting</t>
+          <t>stitch</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>stinging</t>
+          <t>stitches</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -8232,14 +8232,14 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>sting</t>
+          <t>stitch</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>stings</t>
+          <t>stitching</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -8249,14 +8249,14 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>sting</t>
+          <t>stitch</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>stitch</t>
+          <t>stung</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -8266,14 +8266,14 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>stitch</t>
+          <t>sting</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>stitched</t>
+          <t>suffer</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
@@ -8283,14 +8283,14 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>stitch</t>
+          <t>suffer</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>stitches</t>
+          <t>suffered</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
@@ -8300,14 +8300,14 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>stitch</t>
+          <t>suffer</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>stitching</t>
+          <t>suffering</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -8317,14 +8317,14 @@
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>stitch</t>
+          <t>suffer</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>stung</t>
+          <t>suffering</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -8334,14 +8334,14 @@
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>sting</t>
+          <t>suffering</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>suffer</t>
+          <t>sufferings</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -8351,14 +8351,14 @@
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>suffer</t>
+          <t>suffering</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>suffered</t>
+          <t>suffers</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -8375,7 +8375,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>suffering</t>
+          <t>thermalgesia</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -8385,14 +8385,14 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>suffer</t>
+          <t>thermalgesia</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>suffering</t>
+          <t>thermalgesias</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -8402,14 +8402,14 @@
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>suffering</t>
+          <t>thermalgesia</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>sufferings</t>
+          <t>throb</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -8419,14 +8419,14 @@
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>suffering</t>
+          <t>throb</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>suffers</t>
+          <t>throbbed</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -8436,14 +8436,14 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>suffer</t>
+          <t>throb</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>thermalgesia</t>
+          <t>throbbing</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -8453,14 +8453,14 @@
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>thermalgesia</t>
+          <t>throb</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>thermalgesias</t>
+          <t>throbs</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -8470,14 +8470,14 @@
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>thermalgesia</t>
+          <t>throb</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>throb</t>
+          <t>torture</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -8487,14 +8487,14 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>throb</t>
+          <t>torture</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>throbbed</t>
+          <t>tortured</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -8504,14 +8504,14 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>throb</t>
+          <t>torture</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>throbbing</t>
+          <t>tortures</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -8521,14 +8521,14 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>throb</t>
+          <t>torture</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>throbs</t>
+          <t>torturing</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -8538,14 +8538,14 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>throb</t>
+          <t>torture</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>torture</t>
+          <t>twinge</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -8555,14 +8555,14 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>torture</t>
+          <t>twinge</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>tortured</t>
+          <t>twingeing</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -8572,14 +8572,14 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>torture</t>
+          <t>twinge</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>tortures</t>
+          <t>twinges</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -8589,14 +8589,14 @@
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>torture</t>
+          <t>twinge</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>torturing</t>
+          <t>ulalgia</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
@@ -8606,14 +8606,14 @@
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>torture</t>
+          <t>ulalgia</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>twinge</t>
+          <t>ulalgias</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
@@ -8623,14 +8623,14 @@
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>twinge</t>
+          <t>ulalgia</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>twingeing</t>
+          <t>urodynia</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -8640,14 +8640,14 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>twinge</t>
+          <t>urodynia</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>twinges</t>
+          <t>urodynias</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
@@ -8657,82 +8657,82 @@
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>twinge</t>
+          <t>urodynia</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>ulalgia</t>
+          <t>asleep</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>Pain</t>
+          <t>Sleep</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>ulalgia</t>
+          <t>asleep</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>ulalgias</t>
+          <t>bundle</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>Pain</t>
+          <t>Sleep</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>ulalgia</t>
+          <t>bundle</t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>urodynia</t>
+          <t>bundled</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Pain</t>
+          <t>Sleep</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>urodynia</t>
+          <t>bundle</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>urodynias</t>
+          <t>bundles</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Pain</t>
+          <t>Sleep</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>urodynia</t>
+          <t>bundle</t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>asleep</t>
+          <t>bundling</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -8742,14 +8742,14 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>asleep</t>
+          <t>bundle</t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>bundle</t>
+          <t>estivate</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
@@ -8759,14 +8759,14 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>bundle</t>
+          <t>estivate</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>bundled</t>
+          <t>estivated</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
@@ -8776,14 +8776,14 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>bundle</t>
+          <t>estivate</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>bundles</t>
+          <t>estivates</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
@@ -8793,14 +8793,14 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>bundle</t>
+          <t>estivate</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>bundling</t>
+          <t>estivating</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
@@ -8810,14 +8810,14 @@
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>bundle</t>
+          <t>estivate</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>estivate</t>
+          <t>hibernate</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
@@ -8827,14 +8827,14 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>estivate</t>
+          <t>hibernate</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>estivated</t>
+          <t>hibernated</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
@@ -8844,14 +8844,14 @@
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>estivate</t>
+          <t>hibernate</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>estivates</t>
+          <t>hibernates</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
@@ -8861,14 +8861,14 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>estivate</t>
+          <t>hibernate</t>
         </is>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>estivating</t>
+          <t>hibernating</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
@@ -8878,14 +8878,14 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>estivate</t>
+          <t>hibernate</t>
         </is>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>hibernate</t>
+          <t>kip</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
@@ -8895,14 +8895,14 @@
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>hibernate</t>
+          <t>kip</t>
         </is>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>hibernated</t>
+          <t>kipped</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
@@ -8912,14 +8912,14 @@
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>hibernate</t>
+          <t>kip</t>
         </is>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>hibernates</t>
+          <t>kipping</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
@@ -8929,14 +8929,14 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>hibernate</t>
+          <t>kip</t>
         </is>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>hibernating</t>
+          <t>kips</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
@@ -8946,14 +8946,14 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>hibernate</t>
+          <t>kip</t>
         </is>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>kip</t>
+          <t>nap</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
@@ -8963,14 +8963,14 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>kip</t>
+          <t>nap</t>
         </is>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>kipped</t>
+          <t>napped</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
@@ -8980,14 +8980,14 @@
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>kip</t>
+          <t>nap</t>
         </is>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>kipping</t>
+          <t>napping</t>
         </is>
       </c>
       <c r="B504" t="inlineStr">
@@ -8997,14 +8997,14 @@
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>kip</t>
+          <t>nap</t>
         </is>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>kips</t>
+          <t>naps</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
@@ -9014,14 +9014,14 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>kip</t>
+          <t>nap</t>
         </is>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>nap</t>
+          <t>shuteye</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
@@ -9031,14 +9031,14 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>nap</t>
+          <t>shuteye</t>
         </is>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>napped</t>
+          <t>shuteyes</t>
         </is>
       </c>
       <c r="B507" t="inlineStr">
@@ -9048,14 +9048,14 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>nap</t>
+          <t>shuteye</t>
         </is>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>napping</t>
+          <t>sleep</t>
         </is>
       </c>
       <c r="B508" t="inlineStr">
@@ -9065,14 +9065,14 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>nap</t>
+          <t>sleep</t>
         </is>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>naps</t>
+          <t>sleeping</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
@@ -9082,14 +9082,14 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>nap</t>
+          <t>sleep</t>
         </is>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>shuteye</t>
+          <t>sleeping</t>
         </is>
       </c>
       <c r="B510" t="inlineStr">
@@ -9099,14 +9099,14 @@
       </c>
       <c r="C510" t="inlineStr">
         <is>
-          <t>shuteye</t>
+          <t>sleeping</t>
         </is>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>shuteyes</t>
+          <t>sleepings</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
@@ -9116,14 +9116,14 @@
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>shuteye</t>
+          <t>sleeping</t>
         </is>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>sleep</t>
+          <t>sleeps</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
@@ -9140,7 +9140,7 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>sleeping</t>
+          <t>slept</t>
         </is>
       </c>
       <c r="B513" t="inlineStr">
@@ -9149,74 +9149,6 @@
         </is>
       </c>
       <c r="C513" t="inlineStr">
-        <is>
-          <t>sleep</t>
-        </is>
-      </c>
-    </row>
-    <row r="514">
-      <c r="A514" t="inlineStr">
-        <is>
-          <t>sleeping</t>
-        </is>
-      </c>
-      <c r="B514" t="inlineStr">
-        <is>
-          <t>Sleep</t>
-        </is>
-      </c>
-      <c r="C514" t="inlineStr">
-        <is>
-          <t>sleeping</t>
-        </is>
-      </c>
-    </row>
-    <row r="515">
-      <c r="A515" t="inlineStr">
-        <is>
-          <t>sleepings</t>
-        </is>
-      </c>
-      <c r="B515" t="inlineStr">
-        <is>
-          <t>Sleep</t>
-        </is>
-      </c>
-      <c r="C515" t="inlineStr">
-        <is>
-          <t>sleeping</t>
-        </is>
-      </c>
-    </row>
-    <row r="516">
-      <c r="A516" t="inlineStr">
-        <is>
-          <t>sleeps</t>
-        </is>
-      </c>
-      <c r="B516" t="inlineStr">
-        <is>
-          <t>Sleep</t>
-        </is>
-      </c>
-      <c r="C516" t="inlineStr">
-        <is>
-          <t>sleep</t>
-        </is>
-      </c>
-    </row>
-    <row r="517">
-      <c r="A517" t="inlineStr">
-        <is>
-          <t>slept</t>
-        </is>
-      </c>
-      <c r="B517" t="inlineStr">
-        <is>
-          <t>Sleep</t>
-        </is>
-      </c>
-      <c r="C517" t="inlineStr">
         <is>
           <t>sleep</t>
         </is>

</xml_diff>